<commit_message>
Add genetic algorithm Excel example. Updated Matlab plot code
</commit_message>
<xml_diff>
--- a/Lectures/Ex8-4-1.xlsx
+++ b/Lectures/Ex8-4-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Classes\CEE6410\Fall2020\CEE6410-Rosenberg-GitHub\CEE-6410-Rosenberg\Lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA19FFF1-5F33-4EEE-B03B-69F07D1BD2A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFB528B-4B0F-4FED-A77F-66140E241D39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'Gradient-42'!$I$24</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Gradient-6'!$I$21</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">Linearized!$B$35:$K$35</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Linearized!$B$36:$K$36</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">NonlinearSolver!$B$20:$C$20</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
@@ -88,7 +88,7 @@
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'Gradient-42'!$J$24</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Gradient-6'!$J$21</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">Linearized!$B$36</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Linearized!$B$37</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">NonlinearSolver!$B$21</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="118">
   <si>
     <t>Constraint</t>
   </si>
@@ -2496,22 +2496,6 @@
   </si>
   <si>
     <r>
-      <t>j = 1 to 4 piecewise variables for X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Where X</t>
     </r>
     <r>
@@ -3016,6 +3000,21 @@
       </rPr>
       <t>i2</t>
     </r>
+  </si>
+  <si>
+    <t>Wik = integer variable that takes the value 1 when Xk is on that interval, 0 otherwise</t>
+  </si>
+  <si>
+    <t>dmik = left hand side contraint coefficient for constraint m, piecewise index I, and decision variable k</t>
+  </si>
+  <si>
+    <t>emk = left hand side constraint coefficient for constraint m, original decision variable k</t>
+  </si>
+  <si>
+    <t>gradient search optimal point</t>
+  </si>
+  <si>
+    <t>(3) by X2 only</t>
   </si>
 </sst>
 </file>
@@ -3790,7 +3789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4015,6 +4014,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4096,9 +4107,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4108,13 +4116,7 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6690,6 +6692,204 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>479169</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>26022</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160976</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>124611</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:aink="http://schemas.microsoft.com/office/drawing/2016/ink" Requires="xdr14 aink">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53AEB45-5DD2-4E20-9C6F-23980CC4952D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6939360" y="384610"/>
+            <a:ext cx="2735410" cy="2261325"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Ink 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F53AEB45-5DD2-4E20-9C6F-23980CC4952D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6921300" y="278378"/>
+              <a:ext cx="2771169" cy="2473435"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>296449</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>30291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>545751</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>143799</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="18" name="Ink 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1B04EB-4F53-41E8-9DFE-89CB5697D4E8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6145920" y="209585"/>
+            <a:ext cx="3913625" cy="1889640"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="18" name="Ink 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1B04EB-4F53-41E8-9DFE-89CB5697D4E8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6137257" y="200735"/>
+              <a:ext cx="3931312" cy="1906986"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-10-05T17:00:11.684"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.1" units="cm"/>
+      <inkml:brushProperty name="height" value="0.6" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+      <inkml:brushProperty name="inkEffects" value="pencil"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">301 4331,'0'-3,"0"-3,0-4,0-2,3-2,3-5,1-1,-1-2,1 2,0 1,1 2,1 1,0 1,-2 0,1-1,-2 1,-1-1,1 1,0-1,-2 0,1 0,3-2,3-2,1 1,2-2,4-1,3-1,5-5,2-4,5 0,1-2,1-2,-3 2,-2 4,-6 2,-2 5,-4 2,0-1,-4 0,2 4,0 0,3 0,1-2,2-4,6-2,2-3,0 2,0 2,-4 2,-2 3,2 0,2-3,-1 0,0 4,-5 0,0-2,-2-1,2 2,-1 0,-2-1,2-2,3-3,-1 3,1 0,2-1,0 0,2-3,2-3,-1-2,2 2,4-1,4-2,2 0,1 0,-5 3,-3 3,-8 5,-5 5,-1 3,-2 2,0 2,3 3,8-3,5-2,6-1,3-5,5-4,0-5,-3 1,-1 2,-6 2,-7 4,-5 7,-5 3,-6 2,0 1,2 0,1-4,1-1,6-3,16-7,9-8,11-4,13-6,11-3,-1-2,-3 3,-6 5,-14 5,-14 8,-13 8,-10 3,-2 5,-2 2,0 2,4-1,1 0,0 0,0 1,-2-3,0 1,-1-2,-2-1,-1 2,1 1,7 2,11-5,11-6,5-7,12-2,3 3,-5 4,-9 4,-10 5,-8 3,-8 3,-5 0,-5 1,-1 0,0-1,5 1,9 0,9-1,8 0,10 0,4-3,3 0,-5 0,-8 0,-10 1,-9 1,-9-3,-5 1,-4-1,1 1,3 1,8 1,10 1,10 0,6 0,5 0,0 0,-4 0,-7 0,-6 0,-7 0,-3 0,0 0,-1 0,-1 0,6 0,7 0,4 0,-4 0,0 0,-3 0,-6 0,-5 0,-6 0,-3 0,-4 0,2 0,3 0,6 0,8 0,6 0,2 0,1 0,2 0,-6 0,-3 0,0 0,1 0,2 0,0 0,-5 0,-3 0,-3 0,-3 0,-2 0,-1 0,-1 0,-1 0,-3 0,2 0,2 0,6 0,3 0,1 0,-1 0,-4 0,-4 0,-3 0,-3 0,-1 0,2 0,3 0,3 0,3 0,3-2,3-2,1 1,1 0,2 1,3 0,2 2,-4 0,-2 0,-2 0,-5 0,-4 0,-4 0,-3 0,-2 0,-1 0,0 0,2 0,1 0,3 0,1 0,-2 0,-1 0,-1 0,-1 0,-1 0,0 0,-1 0,1 0,-1 0,3 0,1 0,-1 0,-5 0,-8-2,-7-2,-6 1,-7-3,-4 1,-1 0,1 2,2-2,3 0,0-2,-2-4,1-4,1-2,3-1,3 1,-3 2,4 4,8 10,7 7,4 3,3-1,2 2,0-1,0 0,0-1,-4 1,0-1,-1 0,1 2,1-1,-2 1,-4 4,-2 5,-3 5,-1 4,-2-1,-3-5,-1-3,-5-2,-4-1,-2-2,-1 1,-1-2,3-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5754.287">4897 1128,'0'-5,"0"-10,0-9,0-4,0-9,0-6,0-6,0-4,0 0,3 0,1 5,-1 4,0 5,-1 3,2 5,0 6,-1 1,0 2,-2 2,0-1,0 1,-1 0,0 2,0 0,0 2,-1 0,1 0,0 0,0 1,0-1,0 3</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7034.583">4889 257,'-3'0,"-3"3,-6 3,-4 3,-7 4,1 1,1-1,4-8,16-14,16-15,15-15,11-6,12-3,2 0,-3 7,-8 7,-9 12,-10 12,-9 12,-8 9,-5 7,-3 5,-2 4,0 0,0-1,1-4,2 1,2-1,0-1,0-2,-1-5</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="40359.228">301 4236,'0'2,"0"7,0 7,0 4,0 1,-3 2,-3 0,0 1,-3 3,1-2,-1-1,1 0,-1-2,1-1,3-1,-2-3,1 0,2-1,-2-3,1 2,-2 3,1 2,0 5,3 9,1 8,0 6,2 1,0 1,0-4,0-7,1-4,-1-5,0-3,-2 2,-2 2,1 3,1 2,0 2,1 6,0 4,1-2,0-2,0-7,0-6,0-7,0-3,0-4,0 1,0 1,0-2,-2 3,-2 6,1 4,-3-1,1-2,0-3,2-4,0-1,2-2,-2-4,0 2,0 0,0 4,2 0,0 4,-2-3,-1-2,-2 1,0 0,0 3,0 2,0 0,-1 2,-3 1,1-1,2-2,2-3,0-2,0-1,1-2,1 0,2 2,0 1,-2 3,-3-1,-1 0,1-4</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-10-05T17:00:00.553"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">2126 72,'16'319,"-16"4061,6-4170,-4-207,-1-1,1 0,0 1,0-1,0 0,1 0,-1 0,0 0,1-1,-1 1,1-1,0 1,-1-1,1 0,0 0,0 0,0 0,0-1,0 1,-1-1,1 0,0 0,0 0,0 0,0 0,1-1,10 2,586 33,150-30,-451-5,1980 0,-943 87,193-46,-1110-24,817-17,-1231 1,45-4,-58-30,-203-165,181 173,7 6,38 24,300 126,-313-129,1 0,0 0,-1 0,1 0,-1 1,1-1,-1 1,0-1,1 1,-1 0,0 0,0 0,0 0,-1 0,1 1,0-1,-1 1,1-1,-1 1,0-1,0 1,0 0,0-1,0 1,-1 0,1 0,-1 0,0 0,0-1,0 1,0 0,0 0,-1 0,1 0,-1 0,0-1,1 1,-1 0,-1-1,1 1,0 0,-1-1,1 0,-1 1,0-1,1 0,-1 0,0 0,-1 1,-268 178,253-182,8-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2450.618">2181 0,'-80'69,"-126"177,191-236,43-55,172-141,-198 184,-1 0,1 0,0 0,1 0,-1 0,0 0,0 1,1-1,-1 1,1 0,-1-1,1 1,-1 0,1 1,0-1,0 0,-1 1,1 0,0-1,0 1,0 0,-1 1,1-1,0 0,0 1,-1-1,1 1,0 0,-1 0,1 0,-1 1,1-1,-1 0,1 1,-1 0,0-1,0 1,0 0,0 0,0 0,0 1,0-1,0 2,145 195,-123-174</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="26170.206">3336 4260,'3679'0,"-3648"0,0-1,1-2,-2-1,1-2,0-1,22-8,-13 0,-1-1,-1-2,0-2,-2-1,29-22,170-230,-204 240,69-72,-5-5,76-114,-24-32,-84 123,-6-2,-5-3,-6-2,-7-2,-4-9,-34 151,52-307,33-210,-42 463,-38 49,-1-1,-1 1,1-1,-1 0,0-1,-1 1,1-1,-1 1,0-1,-1 0,0 0,0 0,0-1,-1 1,0 0,0-1,-1-1,2-5,49-495,-33-17,-19 527,1 0,-1-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,0-1,1 1,-1-1,0 0,1 1,-1-1,0 0,1 1,-1-1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0-1,1 1,-1 0,0-1,1 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,0 0,-1 0,1 1,0-1,0 0,-1 1,1-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,-50 60,41-48,-13 15,289-239,-265 212,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 1,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 1,0 0,0 0,0 0,0-1,0 2,-1-1,1 0,0 0,-1 1,1-1,-1 0,1 1,-1 0,1-1,-1 1,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 2,4 11,41 139,-36-128</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83726.002">196 4881,'25'-283,"-19"-27,8-326,10 194,3 91,32 42,1 106,60-88,52-58,-167 337,-4 4,1 0,0 1,1 0,-1-1,2 1,-1 0,0 0,1 1,1-1,-1 1,1 0,0 0,0 0,1 1,-1 0,1 0,0 0,1 1,-1 0,1 0,0 0,0 1,0 0,0 1,0-1,3 1,3-1,-1 0,0 1,1 1,0 0,-1 0,1 1,0 1,-1 1,1-1,-1 2,0 0,1 0,-1 1,0 1,-1 0,1 1,-1 0,0 0,-1 1,0 1,0 0,0 0,4 6,37 130,-17-30,149 335,-13-59,-158-357,0-1,2 0,2-1,1 0,1-1,1-2,2 0,1-1,0-1,2-1,1-1,1-1,1-1,1-2,1-1,0-1,2-2,0-1,0-1,10 2,-31-12,0-1,0 0,0-1,0 0,1 0,-1-1,1 0,-1-1,0 0,1-1,-1 0,1-1,-1 0,0 0,0-1,0-1,0 0,-1 0,1-1,-1 0,0 0,6-7,44-40,-2-3,-3-2,-2-3,35-53,106-264,-180 357,63-93,-5-4,41-94,63-161,-162 352,61-88,-5-2,-5-3,46-113,91-333,-140 366,-10 50,-52 143,1 0,-1 1,0-1,1 0,-1 1,0-1,1 0,-1 0,0 0,0 0,1 1,-1-1,0 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0-1,1 1,-1 0,0-1,1 1,-1 0,0-1,1 1,-1-1,1 1,-1-1,0 1,1-1,0 0,-1 1,1-1,-1 0,1 1,0-1,-1 0,1 1,0-1,0 0,0 0,-1 1,1-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,1-1,-1 0,0 0,0 1,1-1,-1 0,0 1,1-1,-1 0,1 0,-61 33,58-31,-117 90,120-91,0-1,-1 1,1-1,-1 0,1 1,-1-1,1 1,-1-1,1 0,-1 1,1-1,-1 0,0 0,0 1,1-1,-1 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-1 1,1-1,0 0,-1 0,1 1,0-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-1 1,0-1,1 1,-1-1,1 1,-1 0,0-1,0 1,1 0,-1-1,0 1,0 0,1 0,-1 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 1,0-1,9-9,1 2,1-1,-1 1,1 0,0 1,1 0,-1 1,1 0,0 0,0 1,1 1,5-1,-13 6,-1 0,-1 1,1 0,0-1,-1 1,1 0,-1 0,0 0,0 1,0-1,0 1,-1-1,1 1,-1-1,0 1,0 0,0-1,-1 1,1 0,-1 0,0 0,0 0,0-1,-1 1,1 0,-1 0,-1 3,2 7,4 40,-1-34</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="85656.26">1 4701,'13'3,"0"0,0 1,0 1,-1 0,0 1,1 0,-2 0,1 2,-1-1,0 1,-1 1,5 5,-6-7,14 16,-22-21,0-1,-1 1,1 0,0-1,0 1,0-1,0 1,1-1,-1 0,0 1,0-1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1-1,0 1,-1 0,1-1,0 0,0 1,-1-1,1 0,0 0,0 0,0 0,-1 0,1 0,0 0,0-1,-1 1,1-1,0 1,-1-1,1 0,0 1,-1-1,1 0,-1 0,1 0,-1-1,0 1,1 0,-1 0,1-2,270-327,-256 314</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="94050.831">783 2670,'319'-32,"775"32,-525-59,-201-37,-47 15,-209 27,-105 48</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6955,8 +7155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB57"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7168,53 +7368,53 @@
       <c r="AB13" s="35"/>
     </row>
     <row r="14" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="87"/>
+      <c r="C14" s="91"/>
       <c r="D14" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="88" t="s">
+      <c r="E14" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="88"/>
+      <c r="F14" s="92"/>
       <c r="G14" s="24" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="24"/>
-      <c r="I14" s="89" t="s">
+      <c r="I14" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="90" t="s">
+      <c r="J14" s="93"/>
+      <c r="K14" s="93"/>
+      <c r="L14" s="93"/>
+      <c r="M14" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="91" t="s">
+      <c r="N14" s="94"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="94"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="S14" s="92"/>
-      <c r="T14" s="92"/>
-      <c r="U14" s="92"/>
-      <c r="V14" s="93"/>
-      <c r="W14" s="82" t="s">
+      <c r="S14" s="96"/>
+      <c r="T14" s="96"/>
+      <c r="U14" s="96"/>
+      <c r="V14" s="97"/>
+      <c r="W14" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="X14" s="83"/>
-      <c r="Y14" s="83"/>
-      <c r="Z14" s="84"/>
+      <c r="X14" s="87"/>
+      <c r="Y14" s="87"/>
+      <c r="Z14" s="88"/>
     </row>
     <row r="15" spans="1:28" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.65">
-      <c r="A15" s="86"/>
+      <c r="A15" s="90"/>
       <c r="B15" s="19" t="s">
         <v>65</v>
       </c>
@@ -8139,16 +8339,16 @@
       <c r="AA46" s="8"/>
     </row>
     <row r="47" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="85" t="s">
+      <c r="A47" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="85"/>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="85"/>
-      <c r="H47" s="85"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="89"/>
+      <c r="E47" s="89"/>
+      <c r="F47" s="89"/>
+      <c r="G47" s="89"/>
+      <c r="H47" s="89"/>
       <c r="AA47" s="8"/>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.35">
@@ -8322,15 +8522,15 @@
     </row>
     <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="61"/>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="101"/>
-      <c r="D13" s="94" t="s">
+      <c r="C13" s="105"/>
+      <c r="D13" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="95"/>
-      <c r="F13" s="96"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="100"/>
     </row>
     <row r="14" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="62" t="s">
@@ -8342,9 +8542,9 @@
       <c r="C14" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="97"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="99"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="103"/>
     </row>
     <row r="15" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="63" t="s">
@@ -8679,53 +8879,53 @@
       <c r="AB13" s="35"/>
     </row>
     <row r="14" spans="1:28" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="86" t="s">
+      <c r="A14" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="87"/>
+      <c r="C14" s="91"/>
       <c r="D14" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="88" t="s">
+      <c r="E14" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="88"/>
+      <c r="F14" s="92"/>
       <c r="G14" s="24" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="24"/>
-      <c r="I14" s="89" t="s">
+      <c r="I14" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="90" t="s">
+      <c r="J14" s="93"/>
+      <c r="K14" s="93"/>
+      <c r="L14" s="93"/>
+      <c r="M14" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="91" t="s">
+      <c r="N14" s="94"/>
+      <c r="O14" s="94"/>
+      <c r="P14" s="94"/>
+      <c r="Q14" s="94"/>
+      <c r="R14" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="S14" s="92"/>
-      <c r="T14" s="92"/>
-      <c r="U14" s="92"/>
-      <c r="V14" s="93"/>
-      <c r="W14" s="82" t="s">
+      <c r="S14" s="96"/>
+      <c r="T14" s="96"/>
+      <c r="U14" s="96"/>
+      <c r="V14" s="97"/>
+      <c r="W14" s="86" t="s">
         <v>79</v>
       </c>
-      <c r="X14" s="83"/>
-      <c r="Y14" s="83"/>
-      <c r="Z14" s="84"/>
+      <c r="X14" s="87"/>
+      <c r="Y14" s="87"/>
+      <c r="Z14" s="88"/>
     </row>
     <row r="15" spans="1:28" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.65">
-      <c r="A15" s="86"/>
+      <c r="A15" s="90"/>
       <c r="B15" s="41" t="s">
         <v>65</v>
       </c>
@@ -9961,16 +10161,16 @@
       <c r="AA49" s="8"/>
     </row>
     <row r="50" spans="1:27" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="85" t="s">
+      <c r="A50" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="85"/>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
-      <c r="E50" s="85"/>
-      <c r="F50" s="85"/>
-      <c r="G50" s="85"/>
-      <c r="H50" s="85"/>
+      <c r="B50" s="89"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="89"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89"/>
+      <c r="G50" s="89"/>
+      <c r="H50" s="89"/>
       <c r="AA50" s="8"/>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.35">
@@ -10076,10 +10276,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:K35"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10087,69 +10287,67 @@
     <col min="1" max="1" width="22.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="17.5" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="G16" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -10159,12 +10357,20 @@
     </row>
     <row r="18" spans="1:14" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="G18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="G19" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A21" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="7">
         <v>0</v>
@@ -10204,23 +10410,23 @@
     </row>
     <row r="23" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="56"/>
-      <c r="B23" s="102" t="s">
+      <c r="B23" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="103"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="103"/>
-      <c r="K23" s="104"/>
-      <c r="L23" s="105" t="s">
+      <c r="C23" s="107"/>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="107"/>
+      <c r="K23" s="108"/>
+      <c r="L23" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="M23" s="106"/>
-      <c r="N23" s="107"/>
+      <c r="M23" s="110"/>
+      <c r="N23" s="111"/>
     </row>
     <row r="24" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="57" t="s">
@@ -10256,33 +10462,33 @@
       <c r="K24" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="L24" s="97"/>
-      <c r="M24" s="98"/>
-      <c r="N24" s="108"/>
+      <c r="L24" s="101"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="112"/>
     </row>
     <row r="25" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="109"/>
-      <c r="B25" s="110" t="s">
+      <c r="A25" s="82"/>
+      <c r="B25" s="113" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="114"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="111"/>
-      <c r="D25" s="111"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="110" t="s">
-        <v>109</v>
-      </c>
-      <c r="G25" s="111"/>
-      <c r="H25" s="111"/>
-      <c r="I25" s="112"/>
-      <c r="J25" s="113"/>
-      <c r="K25" s="113"/>
-      <c r="L25" s="114"/>
-      <c r="M25" s="114"/>
-      <c r="N25" s="115"/>
+      <c r="G25" s="114"/>
+      <c r="H25" s="114"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="83"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="85"/>
     </row>
     <row r="26" spans="1:14" ht="33" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="2">
         <f>B21*(5-B21^2)</f>
@@ -10347,8 +10553,8 @@
         <v>4</v>
       </c>
       <c r="L27" s="54">
-        <f>SUMPRODUCT(B27:K27,$B$35:$K$35)</f>
-        <v>0</v>
+        <f>SUMPRODUCT(B27:K27,$B$36:$K$36)</f>
+        <v>5</v>
       </c>
       <c r="M27" s="54" t="s">
         <v>14</v>
@@ -10376,8 +10582,8 @@
         <v>2</v>
       </c>
       <c r="L28" s="81">
-        <f t="shared" ref="L28:L33" si="2">SUMPRODUCT(B28:K28,$B$35:$K$35)</f>
-        <v>0</v>
+        <f t="shared" ref="L28:L34" si="2">SUMPRODUCT(B28:K28,$B$36:$K$36)</f>
+        <v>8</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>14</v>
@@ -10413,8 +10619,8 @@
       <c r="J29" s="52"/>
       <c r="K29" s="52"/>
       <c r="L29" s="54">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>SUMPRODUCT(B29:K29,$B$36:$K$36)</f>
+        <v>1</v>
       </c>
       <c r="M29" s="54" t="s">
         <v>14</v>
@@ -10425,7 +10631,7 @@
     </row>
     <row r="30" spans="1:14" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -10447,7 +10653,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="81">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>15</v>
@@ -10458,7 +10664,7 @@
     </row>
     <row r="31" spans="1:14" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" s="76" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
@@ -10480,7 +10686,7 @@
       <c r="K31" s="52"/>
       <c r="L31" s="54">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="54" t="s">
         <v>15</v>
@@ -10514,7 +10720,7 @@
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="81">
-        <f>SUMPRODUCT(B32:K32,$B$35:$K$35)</f>
+        <f>SUMPRODUCT(B32:K32,$B$36:$K$36)</f>
         <v>0</v>
       </c>
       <c r="M32" s="3" t="s">
@@ -10559,39 +10765,83 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="47" t="s">
+    <row r="34" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="116" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="116"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="116"/>
+      <c r="N34" s="116"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A36" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
+      <c r="B36" s="49">
+        <v>0</v>
+      </c>
+      <c r="C36" s="49">
+        <v>1</v>
+      </c>
+      <c r="D36" s="49">
+        <v>0</v>
+      </c>
+      <c r="E36" s="49">
+        <v>0</v>
+      </c>
+      <c r="F36" s="49">
+        <v>0</v>
+      </c>
+      <c r="G36" s="49">
+        <v>1</v>
+      </c>
+      <c r="H36" s="49">
+        <v>0</v>
+      </c>
+      <c r="I36" s="49">
+        <v>0</v>
+      </c>
+      <c r="J36" s="49">
+        <v>1</v>
+      </c>
+      <c r="K36" s="49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A37" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="48">
-        <f>SUMPRODUCT(B26:K26,B35:K35)</f>
-        <v>0</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
+      <c r="B37" s="48">
+        <f>SUMPRODUCT(B26:K26,B36:K36)</f>
+        <v>12</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="K37" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="L37" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -10601,5 +10851,6 @@
     <mergeCell ref="F25:I25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>